<commit_message>
New template for orders
</commit_message>
<xml_diff>
--- a/resources/Diggers Factory - Orders Template.xlsx
+++ b/resources/Diggers Factory - Orders Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vico/Sites/diggersfactory/api/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vico/Sites/diggers/api/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5050EF6-89E5-1046-AABB-8553E0DFDC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F52ADB3-8465-8642-AD46-1407D2337634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41040" yWindow="620" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -79,13 +79,19 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>test@test.fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +118,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,10 +144,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -156,8 +171,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,26 +491,26 @@
     <col min="1" max="1" width="23.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="2" customWidth="1"/>
-    <col min="4" max="5" width="13.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="2"/>
-    <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="2"/>
-    <col min="10" max="10" width="19.5" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="6" width="13.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="14.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -504,25 +524,28 @@
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3760370260844</v>
       </c>
@@ -535,27 +558,36 @@
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2">
         <v>142548840</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>94300</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E13" s="8"/>
+      <c r="F13" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>